<commit_message>
Starting last set of tests
</commit_message>
<xml_diff>
--- a/test/Region.xlsx
+++ b/test/Region.xlsx
@@ -5,11 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="constructors" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="bad_constructors" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="failure" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="special" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="basic-normal" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="basic-mixed" sheetId="5" state="visible" r:id="rId6"/>
@@ -20,8 +20,8 @@
     <sheet name="extra" sheetId="10" state="visible" r:id="rId11"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">bad_constructors!$A$1:$E$48</definedName>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">constructors!$A$1:$P$55</definedName>
+    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">failure!$A$1:$E$48</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -2045,11 +2045,11 @@
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="6.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="9.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="8.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="11.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="13.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="11.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="13.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="13.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="14.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="12.13"/>
@@ -9027,7 +9027,7 @@
   </sheetPr>
   <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
     </sheetView>
   </sheetViews>
@@ -9037,7 +9037,7 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.02"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.52"/>
   </cols>
@@ -10022,7 +10022,7 @@
   </sheetPr>
   <dimension ref="A1:AMJ24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="3" ySplit="0" topLeftCell="D1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="AG22" activeCellId="0" sqref="AG22"/>

</xml_diff>